<commit_message>
Updated STIG Definition Template
</commit_message>
<xml_diff>
--- a/Toolbx.STIGSupport/tools/STIG Definition - StigName.xlsx
+++ b/Toolbx.STIGSupport/tools/STIG Definition - StigName.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zachary Shupp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zach\OneDrive\Projects\Toolbx.STIGSupport\Toolbx.STIGSupport\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3453F4B3-9A06-4989-9632-5FB61910452C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE1DD53-B193-4B37-A0DD-AB440ABCBC53}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-255" windowWidth="29040" windowHeight="15840" xr2:uid="{F8BA821C-0127-4BCE-88D9-8B02E889E8E8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8BA821C-0127-4BCE-88D9-8B02E889E8E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Exceptions" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>VulnID</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>STIG Defintion:</t>
+  </si>
+  <si>
+    <t>Applies  To</t>
   </si>
 </sst>
 </file>
@@ -205,14 +208,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -531,7 +534,7 @@
   <dimension ref="B2:N101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,17 +549,18 @@
     <col min="9" max="10" width="8.28515625" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.28515625" style="14" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="50.7109375" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="3"/>
+    <col min="13" max="13" width="28.5703125" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
       <c r="G2" s="1"/>
       <c r="H2" s="2"/>
       <c r="I2" s="16"/>
@@ -565,13 +569,13 @@
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
       <c r="G3" s="1"/>
       <c r="H3" s="2"/>
       <c r="I3" s="16"/>
@@ -628,6 +632,9 @@
       <c r="L5" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="M5" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="15"/>
@@ -641,6 +648,7 @@
       <c r="J6" s="12"/>
       <c r="K6" s="11"/>
       <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
@@ -654,6 +662,7 @@
       <c r="J7" s="12"/>
       <c r="K7" s="11"/>
       <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="12"/>
@@ -667,6 +676,7 @@
       <c r="J8" s="12"/>
       <c r="K8" s="11"/>
       <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="12"/>
@@ -680,6 +690,7 @@
       <c r="J9" s="12"/>
       <c r="K9" s="11"/>
       <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="12"/>
@@ -693,6 +704,7 @@
       <c r="J10" s="12"/>
       <c r="K10" s="11"/>
       <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="12"/>
@@ -706,6 +718,7 @@
       <c r="J11" s="12"/>
       <c r="K11" s="11"/>
       <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="12"/>
@@ -719,6 +732,7 @@
       <c r="J12" s="12"/>
       <c r="K12" s="11"/>
       <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="12"/>
@@ -732,6 +746,7 @@
       <c r="J13" s="12"/>
       <c r="K13" s="11"/>
       <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
@@ -745,6 +760,7 @@
       <c r="J14" s="12"/>
       <c r="K14" s="11"/>
       <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="12"/>
@@ -758,6 +774,7 @@
       <c r="J15" s="12"/>
       <c r="K15" s="11"/>
       <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="12"/>
@@ -771,8 +788,9 @@
       <c r="J16" s="12"/>
       <c r="K16" s="11"/>
       <c r="L16" s="10"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="10"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
       <c r="D17" s="11"/>
@@ -784,8 +802,9 @@
       <c r="J17" s="12"/>
       <c r="K17" s="11"/>
       <c r="L17" s="10"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="10"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
       <c r="D18" s="11"/>
@@ -797,8 +816,9 @@
       <c r="J18" s="12"/>
       <c r="K18" s="11"/>
       <c r="L18" s="10"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M18" s="10"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
       <c r="D19" s="11"/>
@@ -810,8 +830,9 @@
       <c r="J19" s="12"/>
       <c r="K19" s="11"/>
       <c r="L19" s="10"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M19" s="10"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
       <c r="D20" s="11"/>
@@ -823,8 +844,9 @@
       <c r="J20" s="12"/>
       <c r="K20" s="11"/>
       <c r="L20" s="10"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M20" s="10"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
       <c r="D21" s="11"/>
@@ -836,8 +858,9 @@
       <c r="J21" s="12"/>
       <c r="K21" s="11"/>
       <c r="L21" s="10"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M21" s="10"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="11"/>
@@ -849,8 +872,9 @@
       <c r="J22" s="12"/>
       <c r="K22" s="11"/>
       <c r="L22" s="10"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M22" s="10"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="11"/>
@@ -862,8 +886,9 @@
       <c r="J23" s="12"/>
       <c r="K23" s="11"/>
       <c r="L23" s="10"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M23" s="10"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="11"/>
@@ -875,8 +900,9 @@
       <c r="J24" s="12"/>
       <c r="K24" s="11"/>
       <c r="L24" s="10"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M24" s="10"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="11"/>
@@ -888,8 +914,9 @@
       <c r="J25" s="12"/>
       <c r="K25" s="11"/>
       <c r="L25" s="10"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M25" s="10"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="11"/>
@@ -901,8 +928,9 @@
       <c r="J26" s="12"/>
       <c r="K26" s="11"/>
       <c r="L26" s="10"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M26" s="10"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="11"/>
@@ -914,8 +942,9 @@
       <c r="J27" s="12"/>
       <c r="K27" s="11"/>
       <c r="L27" s="10"/>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M27" s="10"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="11"/>
@@ -927,8 +956,9 @@
       <c r="J28" s="12"/>
       <c r="K28" s="11"/>
       <c r="L28" s="10"/>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M28" s="10"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="11"/>
@@ -940,8 +970,9 @@
       <c r="J29" s="12"/>
       <c r="K29" s="11"/>
       <c r="L29" s="10"/>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M29" s="10"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
       <c r="D30" s="11"/>
@@ -953,8 +984,9 @@
       <c r="J30" s="12"/>
       <c r="K30" s="11"/>
       <c r="L30" s="10"/>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M30" s="10"/>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
       <c r="D31" s="11"/>
@@ -966,8 +998,9 @@
       <c r="J31" s="12"/>
       <c r="K31" s="11"/>
       <c r="L31" s="10"/>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M31" s="10"/>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
       <c r="D32" s="11"/>
@@ -979,8 +1012,9 @@
       <c r="J32" s="12"/>
       <c r="K32" s="11"/>
       <c r="L32" s="10"/>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M32" s="10"/>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
       <c r="D33" s="11"/>
@@ -992,8 +1026,9 @@
       <c r="J33" s="12"/>
       <c r="K33" s="11"/>
       <c r="L33" s="10"/>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M33" s="10"/>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="11"/>
@@ -1005,8 +1040,9 @@
       <c r="J34" s="12"/>
       <c r="K34" s="11"/>
       <c r="L34" s="10"/>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M34" s="10"/>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="11"/>
@@ -1018,8 +1054,9 @@
       <c r="J35" s="12"/>
       <c r="K35" s="11"/>
       <c r="L35" s="10"/>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M35" s="10"/>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="11"/>
@@ -1031,8 +1068,9 @@
       <c r="J36" s="12"/>
       <c r="K36" s="11"/>
       <c r="L36" s="10"/>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M36" s="10"/>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
       <c r="D37" s="11"/>
@@ -1044,8 +1082,9 @@
       <c r="J37" s="12"/>
       <c r="K37" s="11"/>
       <c r="L37" s="10"/>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M37" s="10"/>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="11"/>
@@ -1057,8 +1096,9 @@
       <c r="J38" s="12"/>
       <c r="K38" s="11"/>
       <c r="L38" s="10"/>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M38" s="10"/>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
       <c r="D39" s="11"/>
@@ -1070,8 +1110,9 @@
       <c r="J39" s="12"/>
       <c r="K39" s="11"/>
       <c r="L39" s="10"/>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M39" s="10"/>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
       <c r="D40" s="11"/>
@@ -1083,8 +1124,9 @@
       <c r="J40" s="12"/>
       <c r="K40" s="11"/>
       <c r="L40" s="10"/>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M40" s="10"/>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
       <c r="D41" s="11"/>
@@ -1096,8 +1138,9 @@
       <c r="J41" s="12"/>
       <c r="K41" s="11"/>
       <c r="L41" s="10"/>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M41" s="10"/>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
       <c r="D42" s="11"/>
@@ -1109,8 +1152,9 @@
       <c r="J42" s="12"/>
       <c r="K42" s="11"/>
       <c r="L42" s="10"/>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M42" s="10"/>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
       <c r="D43" s="11"/>
@@ -1122,8 +1166,9 @@
       <c r="J43" s="12"/>
       <c r="K43" s="11"/>
       <c r="L43" s="10"/>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M43" s="10"/>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
       <c r="D44" s="11"/>
@@ -1135,8 +1180,9 @@
       <c r="J44" s="12"/>
       <c r="K44" s="11"/>
       <c r="L44" s="10"/>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M44" s="10"/>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
       <c r="D45" s="11"/>
@@ -1148,8 +1194,9 @@
       <c r="J45" s="12"/>
       <c r="K45" s="11"/>
       <c r="L45" s="10"/>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M45" s="10"/>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="11"/>
@@ -1161,8 +1208,9 @@
       <c r="J46" s="12"/>
       <c r="K46" s="11"/>
       <c r="L46" s="10"/>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M46" s="10"/>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="11"/>
@@ -1174,8 +1222,9 @@
       <c r="J47" s="12"/>
       <c r="K47" s="11"/>
       <c r="L47" s="10"/>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M47" s="10"/>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="11"/>
@@ -1187,8 +1236,9 @@
       <c r="J48" s="12"/>
       <c r="K48" s="11"/>
       <c r="L48" s="10"/>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M48" s="10"/>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="11"/>
@@ -1200,8 +1250,9 @@
       <c r="J49" s="12"/>
       <c r="K49" s="11"/>
       <c r="L49" s="10"/>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M49" s="10"/>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
       <c r="D50" s="11"/>
@@ -1213,8 +1264,9 @@
       <c r="J50" s="12"/>
       <c r="K50" s="11"/>
       <c r="L50" s="10"/>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M50" s="10"/>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
       <c r="D51" s="11"/>
@@ -1226,8 +1278,9 @@
       <c r="J51" s="12"/>
       <c r="K51" s="11"/>
       <c r="L51" s="10"/>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M51" s="10"/>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
       <c r="D52" s="11"/>
@@ -1239,8 +1292,9 @@
       <c r="J52" s="12"/>
       <c r="K52" s="11"/>
       <c r="L52" s="10"/>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M52" s="10"/>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
       <c r="D53" s="11"/>
@@ -1252,8 +1306,9 @@
       <c r="J53" s="12"/>
       <c r="K53" s="11"/>
       <c r="L53" s="10"/>
-    </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M53" s="10"/>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
       <c r="D54" s="11"/>
@@ -1265,8 +1320,9 @@
       <c r="J54" s="12"/>
       <c r="K54" s="11"/>
       <c r="L54" s="10"/>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M54" s="10"/>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
       <c r="D55" s="11"/>
@@ -1278,8 +1334,9 @@
       <c r="J55" s="12"/>
       <c r="K55" s="11"/>
       <c r="L55" s="10"/>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M55" s="10"/>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
       <c r="D56" s="11"/>
@@ -1291,8 +1348,9 @@
       <c r="J56" s="12"/>
       <c r="K56" s="11"/>
       <c r="L56" s="10"/>
-    </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M56" s="10"/>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
       <c r="D57" s="11"/>
@@ -1304,8 +1362,9 @@
       <c r="J57" s="12"/>
       <c r="K57" s="11"/>
       <c r="L57" s="10"/>
-    </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M57" s="10"/>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
       <c r="D58" s="11"/>
@@ -1317,8 +1376,9 @@
       <c r="J58" s="12"/>
       <c r="K58" s="11"/>
       <c r="L58" s="10"/>
-    </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M58" s="10"/>
+    </row>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
       <c r="D59" s="11"/>
@@ -1330,8 +1390,9 @@
       <c r="J59" s="12"/>
       <c r="K59" s="11"/>
       <c r="L59" s="10"/>
-    </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M59" s="10"/>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B60" s="12"/>
       <c r="C60" s="12"/>
       <c r="D60" s="11"/>
@@ -1343,8 +1404,9 @@
       <c r="J60" s="12"/>
       <c r="K60" s="11"/>
       <c r="L60" s="10"/>
-    </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M60" s="10"/>
+    </row>
+    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B61" s="12"/>
       <c r="C61" s="12"/>
       <c r="D61" s="11"/>
@@ -1356,8 +1418,9 @@
       <c r="J61" s="12"/>
       <c r="K61" s="11"/>
       <c r="L61" s="10"/>
-    </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M61" s="10"/>
+    </row>
+    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B62" s="12"/>
       <c r="C62" s="12"/>
       <c r="D62" s="11"/>
@@ -1369,8 +1432,9 @@
       <c r="J62" s="12"/>
       <c r="K62" s="11"/>
       <c r="L62" s="10"/>
-    </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M62" s="10"/>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B63" s="12"/>
       <c r="C63" s="12"/>
       <c r="D63" s="11"/>
@@ -1382,8 +1446,9 @@
       <c r="J63" s="12"/>
       <c r="K63" s="11"/>
       <c r="L63" s="10"/>
-    </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M63" s="10"/>
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B64" s="12"/>
       <c r="C64" s="12"/>
       <c r="D64" s="11"/>
@@ -1395,8 +1460,9 @@
       <c r="J64" s="12"/>
       <c r="K64" s="11"/>
       <c r="L64" s="10"/>
-    </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M64" s="10"/>
+    </row>
+    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B65" s="12"/>
       <c r="C65" s="12"/>
       <c r="D65" s="11"/>
@@ -1408,8 +1474,9 @@
       <c r="J65" s="12"/>
       <c r="K65" s="11"/>
       <c r="L65" s="10"/>
-    </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M65" s="10"/>
+    </row>
+    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B66" s="12"/>
       <c r="C66" s="12"/>
       <c r="D66" s="11"/>
@@ -1421,8 +1488,9 @@
       <c r="J66" s="12"/>
       <c r="K66" s="11"/>
       <c r="L66" s="10"/>
-    </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M66" s="10"/>
+    </row>
+    <row r="67" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B67" s="12"/>
       <c r="C67" s="12"/>
       <c r="D67" s="11"/>
@@ -1434,8 +1502,9 @@
       <c r="J67" s="12"/>
       <c r="K67" s="11"/>
       <c r="L67" s="10"/>
-    </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M67" s="10"/>
+    </row>
+    <row r="68" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B68" s="12"/>
       <c r="C68" s="12"/>
       <c r="D68" s="11"/>
@@ -1447,8 +1516,9 @@
       <c r="J68" s="12"/>
       <c r="K68" s="11"/>
       <c r="L68" s="10"/>
-    </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M68" s="10"/>
+    </row>
+    <row r="69" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B69" s="12"/>
       <c r="C69" s="12"/>
       <c r="D69" s="11"/>
@@ -1460,8 +1530,9 @@
       <c r="J69" s="12"/>
       <c r="K69" s="11"/>
       <c r="L69" s="10"/>
-    </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M69" s="10"/>
+    </row>
+    <row r="70" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B70" s="12"/>
       <c r="C70" s="12"/>
       <c r="D70" s="11"/>
@@ -1473,8 +1544,9 @@
       <c r="J70" s="12"/>
       <c r="K70" s="11"/>
       <c r="L70" s="10"/>
-    </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M70" s="10"/>
+    </row>
+    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B71" s="12"/>
       <c r="C71" s="12"/>
       <c r="D71" s="11"/>
@@ -1486,8 +1558,9 @@
       <c r="J71" s="12"/>
       <c r="K71" s="11"/>
       <c r="L71" s="10"/>
-    </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M71" s="10"/>
+    </row>
+    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B72" s="12"/>
       <c r="C72" s="12"/>
       <c r="D72" s="11"/>
@@ -1499,8 +1572,9 @@
       <c r="J72" s="12"/>
       <c r="K72" s="11"/>
       <c r="L72" s="10"/>
-    </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M72" s="10"/>
+    </row>
+    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B73" s="12"/>
       <c r="C73" s="12"/>
       <c r="D73" s="11"/>
@@ -1512,8 +1586,9 @@
       <c r="J73" s="12"/>
       <c r="K73" s="11"/>
       <c r="L73" s="10"/>
-    </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M73" s="10"/>
+    </row>
+    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B74" s="12"/>
       <c r="C74" s="12"/>
       <c r="D74" s="11"/>
@@ -1525,8 +1600,9 @@
       <c r="J74" s="12"/>
       <c r="K74" s="11"/>
       <c r="L74" s="10"/>
-    </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M74" s="10"/>
+    </row>
+    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B75" s="12"/>
       <c r="C75" s="12"/>
       <c r="D75" s="11"/>
@@ -1538,8 +1614,9 @@
       <c r="J75" s="12"/>
       <c r="K75" s="11"/>
       <c r="L75" s="10"/>
-    </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M75" s="10"/>
+    </row>
+    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B76" s="12"/>
       <c r="C76" s="12"/>
       <c r="D76" s="11"/>
@@ -1551,8 +1628,9 @@
       <c r="J76" s="12"/>
       <c r="K76" s="11"/>
       <c r="L76" s="10"/>
-    </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M76" s="10"/>
+    </row>
+    <row r="77" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B77" s="12"/>
       <c r="C77" s="12"/>
       <c r="D77" s="11"/>
@@ -1564,8 +1642,9 @@
       <c r="J77" s="12"/>
       <c r="K77" s="11"/>
       <c r="L77" s="10"/>
-    </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M77" s="10"/>
+    </row>
+    <row r="78" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B78" s="12"/>
       <c r="C78" s="12"/>
       <c r="D78" s="11"/>
@@ -1577,8 +1656,9 @@
       <c r="J78" s="12"/>
       <c r="K78" s="11"/>
       <c r="L78" s="10"/>
-    </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M78" s="10"/>
+    </row>
+    <row r="79" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B79" s="12"/>
       <c r="C79" s="12"/>
       <c r="D79" s="11"/>
@@ -1590,8 +1670,9 @@
       <c r="J79" s="12"/>
       <c r="K79" s="11"/>
       <c r="L79" s="10"/>
-    </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M79" s="10"/>
+    </row>
+    <row r="80" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B80" s="12"/>
       <c r="C80" s="12"/>
       <c r="D80" s="11"/>
@@ -1603,8 +1684,9 @@
       <c r="J80" s="12"/>
       <c r="K80" s="11"/>
       <c r="L80" s="10"/>
-    </row>
-    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M80" s="10"/>
+    </row>
+    <row r="81" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B81" s="12"/>
       <c r="C81" s="12"/>
       <c r="D81" s="11"/>
@@ -1616,8 +1698,9 @@
       <c r="J81" s="12"/>
       <c r="K81" s="11"/>
       <c r="L81" s="10"/>
-    </row>
-    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M81" s="10"/>
+    </row>
+    <row r="82" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B82" s="12"/>
       <c r="C82" s="12"/>
       <c r="D82" s="11"/>
@@ -1629,8 +1712,9 @@
       <c r="J82" s="12"/>
       <c r="K82" s="11"/>
       <c r="L82" s="10"/>
-    </row>
-    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M82" s="10"/>
+    </row>
+    <row r="83" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B83" s="12"/>
       <c r="C83" s="12"/>
       <c r="D83" s="11"/>
@@ -1642,8 +1726,9 @@
       <c r="J83" s="12"/>
       <c r="K83" s="11"/>
       <c r="L83" s="10"/>
-    </row>
-    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M83" s="10"/>
+    </row>
+    <row r="84" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B84" s="12"/>
       <c r="C84" s="12"/>
       <c r="D84" s="11"/>
@@ -1655,8 +1740,9 @@
       <c r="J84" s="12"/>
       <c r="K84" s="11"/>
       <c r="L84" s="10"/>
-    </row>
-    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M84" s="10"/>
+    </row>
+    <row r="85" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B85" s="12"/>
       <c r="C85" s="12"/>
       <c r="D85" s="11"/>
@@ -1668,8 +1754,9 @@
       <c r="J85" s="12"/>
       <c r="K85" s="11"/>
       <c r="L85" s="10"/>
-    </row>
-    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M85" s="10"/>
+    </row>
+    <row r="86" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B86" s="12"/>
       <c r="C86" s="12"/>
       <c r="D86" s="11"/>
@@ -1681,8 +1768,9 @@
       <c r="J86" s="12"/>
       <c r="K86" s="11"/>
       <c r="L86" s="10"/>
-    </row>
-    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M86" s="10"/>
+    </row>
+    <row r="87" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B87" s="12"/>
       <c r="C87" s="12"/>
       <c r="D87" s="11"/>
@@ -1694,8 +1782,9 @@
       <c r="J87" s="12"/>
       <c r="K87" s="11"/>
       <c r="L87" s="10"/>
-    </row>
-    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M87" s="10"/>
+    </row>
+    <row r="88" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B88" s="12"/>
       <c r="C88" s="12"/>
       <c r="D88" s="11"/>
@@ -1707,8 +1796,9 @@
       <c r="J88" s="12"/>
       <c r="K88" s="11"/>
       <c r="L88" s="10"/>
-    </row>
-    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M88" s="10"/>
+    </row>
+    <row r="89" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B89" s="12"/>
       <c r="C89" s="12"/>
       <c r="D89" s="11"/>
@@ -1720,8 +1810,9 @@
       <c r="J89" s="12"/>
       <c r="K89" s="11"/>
       <c r="L89" s="10"/>
-    </row>
-    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M89" s="10"/>
+    </row>
+    <row r="90" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B90" s="12"/>
       <c r="C90" s="12"/>
       <c r="D90" s="11"/>
@@ -1733,8 +1824,9 @@
       <c r="J90" s="12"/>
       <c r="K90" s="11"/>
       <c r="L90" s="10"/>
-    </row>
-    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M90" s="10"/>
+    </row>
+    <row r="91" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B91" s="12"/>
       <c r="C91" s="12"/>
       <c r="D91" s="11"/>
@@ -1746,8 +1838,9 @@
       <c r="J91" s="12"/>
       <c r="K91" s="11"/>
       <c r="L91" s="10"/>
-    </row>
-    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M91" s="10"/>
+    </row>
+    <row r="92" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B92" s="12"/>
       <c r="C92" s="12"/>
       <c r="D92" s="11"/>
@@ -1759,8 +1852,9 @@
       <c r="J92" s="12"/>
       <c r="K92" s="11"/>
       <c r="L92" s="10"/>
-    </row>
-    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M92" s="10"/>
+    </row>
+    <row r="93" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B93" s="12"/>
       <c r="C93" s="12"/>
       <c r="D93" s="11"/>
@@ -1772,8 +1866,9 @@
       <c r="J93" s="12"/>
       <c r="K93" s="11"/>
       <c r="L93" s="10"/>
-    </row>
-    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M93" s="10"/>
+    </row>
+    <row r="94" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B94" s="12"/>
       <c r="C94" s="12"/>
       <c r="D94" s="11"/>
@@ -1785,8 +1880,9 @@
       <c r="J94" s="12"/>
       <c r="K94" s="11"/>
       <c r="L94" s="10"/>
-    </row>
-    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M94" s="10"/>
+    </row>
+    <row r="95" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B95" s="12"/>
       <c r="C95" s="12"/>
       <c r="D95" s="11"/>
@@ -1798,8 +1894,9 @@
       <c r="J95" s="12"/>
       <c r="K95" s="11"/>
       <c r="L95" s="10"/>
-    </row>
-    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M95" s="10"/>
+    </row>
+    <row r="96" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B96" s="12"/>
       <c r="C96" s="12"/>
       <c r="D96" s="11"/>
@@ -1811,8 +1908,9 @@
       <c r="J96" s="12"/>
       <c r="K96" s="11"/>
       <c r="L96" s="10"/>
-    </row>
-    <row r="97" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M96" s="10"/>
+    </row>
+    <row r="97" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B97" s="12"/>
       <c r="C97" s="12"/>
       <c r="D97" s="11"/>
@@ -1824,8 +1922,9 @@
       <c r="J97" s="12"/>
       <c r="K97" s="11"/>
       <c r="L97" s="10"/>
-    </row>
-    <row r="98" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M97" s="10"/>
+    </row>
+    <row r="98" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B98" s="12"/>
       <c r="C98" s="12"/>
       <c r="D98" s="11"/>
@@ -1837,8 +1936,9 @@
       <c r="J98" s="12"/>
       <c r="K98" s="11"/>
       <c r="L98" s="10"/>
-    </row>
-    <row r="99" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M98" s="10"/>
+    </row>
+    <row r="99" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B99" s="12"/>
       <c r="C99" s="12"/>
       <c r="D99" s="11"/>
@@ -1850,8 +1950,9 @@
       <c r="J99" s="12"/>
       <c r="K99" s="11"/>
       <c r="L99" s="10"/>
-    </row>
-    <row r="100" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M99" s="10"/>
+    </row>
+    <row r="100" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B100" s="12"/>
       <c r="C100" s="12"/>
       <c r="D100" s="11"/>
@@ -1863,8 +1964,9 @@
       <c r="J100" s="12"/>
       <c r="K100" s="11"/>
       <c r="L100" s="10"/>
-    </row>
-    <row r="101" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M100" s="10"/>
+    </row>
+    <row r="101" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B101" s="12"/>
       <c r="C101" s="12"/>
       <c r="D101" s="11"/>
@@ -1876,6 +1978,7 @@
       <c r="J101" s="12"/>
       <c r="K101" s="11"/>
       <c r="L101" s="10"/>
+      <c r="M101" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="B5:L101" xr:uid="{6A71790B-8135-4ADD-B0FF-EC3EC4B14237}"/>

</xml_diff>